<commit_message>
Fixed errors with merge
</commit_message>
<xml_diff>
--- a/image/activitydefinition.xlsx
+++ b/image/activitydefinition.xlsx
@@ -963,7 +963,7 @@
     <t>ActivityDefinition.intent</t>
   </si>
   <si>
-    <t>proposal | plan | order</t>
+    <t>proposal | plan | directive | order | original-order | reflex-order | filler-order | instance-order | option</t>
   </si>
   <si>
     <t>Indicates the level of authority/intentionality associated with the activity and where the request should fit into the workflow chain.</t>
@@ -1485,7 +1485,7 @@
     <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="86.45703125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="93.171875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>

</xml_diff>